<commit_message>
Added: Logs, resources, SearchCharacterViaSearchTest
</commit_message>
<xml_diff>
--- a/resources/testdata.xlsx
+++ b/resources/testdata.xlsx
@@ -16,13 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
-  <si>
-    <t>browser</t>
-  </si>
-  <si>
-    <t>runmode</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="16">
   <si>
     <t>chrome</t>
   </si>
@@ -34,6 +28,42 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Spiderman</t>
+  </si>
+  <si>
+    <t>Mantis</t>
+  </si>
+  <si>
+    <t>Swordsman</t>
+  </si>
+  <si>
+    <t>Turbo</t>
+  </si>
+  <si>
+    <t>Helix</t>
+  </si>
+  <si>
+    <t>Jessica Jones</t>
+  </si>
+  <si>
+    <t>Hellstorm</t>
+  </si>
+  <si>
+    <t>browserType</t>
+  </si>
+  <si>
+    <t>executionMode</t>
+  </si>
+  <si>
+    <t>primaryCharacter</t>
+  </si>
+  <si>
+    <t>secondaryCharacter</t>
+  </si>
+  <si>
+    <t>expectedResultCount</t>
   </si>
 </sst>
 </file>
@@ -372,67 +402,208 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="32.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <v>133</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="A2:E5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>